<commit_message>
[IMP] midea backport from 12.0
</commit_message>
<xml_diff>
--- a/test_testenv/tests/data/account_account.xlsx
+++ b/test_testenv/tests/data/account_account.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="98">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -299,6 +299,12 @@
   </si>
   <si>
     <t xml:space="preserve">Dividends</t>
+  </si>
+  <si>
+    <t xml:space="preserve">z0bug.coa_gc_rc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">G/C RC</t>
   </si>
   <si>
     <t xml:space="preserve">z0bug.lp</t>
@@ -541,12 +547,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F38"/>
+  <dimension ref="A1:F39"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A25" activeCellId="0" sqref="A25"/>
+      <selection pane="bottomLeft" activeCell="D38" activeCellId="0" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1197,18 +1203,36 @@
         <v>93</v>
       </c>
       <c r="B38" s="2" t="n">
+        <v>490050</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F38" s="4"/>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="B39" s="2" t="n">
         <v>999999</v>
       </c>
-      <c r="C38" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="D38" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="E38" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F38" s="4"/>
+      <c r="C39" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F39" s="4"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>